<commit_message>
Updated parser and coef in w2n
</commit_message>
<xml_diff>
--- a/Dictionaries/w2n_tokens.xlsx
+++ b/Dictionaries/w2n_tokens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\Documents\GitHub\exchange-rates-tg-bot\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B1C560-8105-407D-833A-883E55428439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC99BAF7-026B-4E43-8B4F-21572B8DB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
   <si>
     <t>token</t>
   </si>
@@ -243,9 +243,6 @@
     <t>тридцять</t>
   </si>
   <si>
-    <t>чотирьохдесят</t>
-  </si>
-  <si>
     <t>п’ятдесят</t>
   </si>
   <si>
@@ -442,6 +439,36 @@
   </si>
   <si>
     <t>двохстами</t>
+  </si>
+  <si>
+    <t>тища</t>
+  </si>
+  <si>
+    <t>пара</t>
+  </si>
+  <si>
+    <t>двох</t>
+  </si>
+  <si>
+    <t>трьох</t>
+  </si>
+  <si>
+    <t>чотирьох</t>
+  </si>
+  <si>
+    <t>п'ятьох</t>
+  </si>
+  <si>
+    <t>шістьох</t>
+  </si>
+  <si>
+    <t>семи</t>
+  </si>
+  <si>
+    <t>сімох</t>
+  </si>
+  <si>
+    <t>восьми</t>
   </si>
 </sst>
 </file>
@@ -759,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:XFD81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +845,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -832,10 +859,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -846,10 +873,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -860,10 +887,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -874,10 +901,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -888,10 +915,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -902,10 +929,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -916,10 +943,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -930,10 +957,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -944,10 +971,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -958,10 +985,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -972,10 +999,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -986,10 +1013,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1000,10 +1027,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1014,10 +1041,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1028,10 +1055,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1042,10 +1069,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1056,10 +1083,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1070,13 +1097,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1084,10 +1111,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1098,10 +1125,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -1112,10 +1139,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1126,10 +1153,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1140,10 +1167,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -1154,10 +1181,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1168,10 +1195,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1182,13 +1209,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1196,10 +1223,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1210,10 +1237,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1224,10 +1251,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B33">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -1238,10 +1265,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B34">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1252,10 +1279,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1266,10 +1293,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -1280,10 +1307,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -1294,10 +1321,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1308,27 +1335,27 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B39">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B40">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1336,13 +1363,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41">
-        <v>1000000000</v>
+        <v>1000000</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1350,13 +1377,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B42">
-        <v>12</v>
+        <v>1000000000</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1364,10 +1391,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1378,7 +1405,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>50</v>
@@ -1392,13 +1419,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1406,7 +1433,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>100</v>
@@ -1420,13 +1447,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B47">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1434,7 +1461,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>1000</v>
@@ -1448,13 +1475,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1462,7 +1489,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>1000000</v>
@@ -1476,24 +1503,24 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1504,10 +1531,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1518,10 +1545,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1532,10 +1559,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1546,10 +1573,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1560,10 +1587,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1574,10 +1601,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1588,10 +1615,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
       <c r="B59">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1602,10 +1629,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B60">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1616,10 +1643,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="B61">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1630,10 +1657,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="B62">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1644,10 +1671,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="B63">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1658,10 +1685,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B64">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1672,10 +1699,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="B65">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1686,10 +1713,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="B66">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1700,10 +1727,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B67">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -1714,10 +1741,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="B68">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1728,10 +1755,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B69">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -1742,10 +1769,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="B70">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -1756,13 +1783,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B71">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -1770,13 +1797,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B72">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1784,13 +1811,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B73">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -1798,13 +1825,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B74">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -1812,13 +1839,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B75">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -1826,13 +1853,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B76">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -1840,13 +1867,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B77">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -1854,13 +1881,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B78">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -1868,13 +1895,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B79">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -1882,13 +1909,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B80">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -1896,13 +1923,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="B81">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -1910,13 +1937,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B82">
-        <v>300</v>
+        <v>40</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -1924,13 +1951,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B83">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="C83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -1938,13 +1965,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B84">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -1952,13 +1979,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B85">
-        <v>600</v>
+        <v>70</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -1966,13 +1993,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B86">
-        <v>700</v>
+        <v>80</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -1980,13 +2007,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B87">
-        <v>800</v>
+        <v>90</v>
       </c>
       <c r="C87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -1994,10 +2021,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="B88">
-        <v>900</v>
+        <v>100</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -2008,55 +2035,55 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B89">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="C89">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="B90">
-        <v>1000000</v>
+        <v>200</v>
       </c>
       <c r="C90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B91">
-        <v>1000000000</v>
+        <v>300</v>
       </c>
       <c r="C91">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -2064,13 +2091,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -2078,13 +2105,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B94">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2092,13 +2119,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B95">
+        <v>700</v>
+      </c>
+      <c r="C95">
         <v>3</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2106,13 +2133,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>800</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2120,13 +2147,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B97">
-        <v>5</v>
+        <v>900</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -2134,66 +2161,66 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="B98">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B99">
-        <v>7</v>
+        <v>1000</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B100">
-        <v>8</v>
+        <v>1000000</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B101">
-        <v>9</v>
+        <v>1000000000</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B102">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -2204,10 +2231,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B103">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -2218,10 +2245,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B104">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -2232,10 +2259,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B105">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -2246,10 +2273,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B106">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -2260,10 +2287,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B107">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -2274,10 +2301,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B108">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -2288,10 +2315,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B109">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -2302,10 +2329,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B110">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -2316,10 +2343,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B111">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2330,13 +2357,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B112">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -2344,13 +2371,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B113">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -2358,13 +2385,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B114">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -2372,13 +2399,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B115">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -2386,13 +2413,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B116">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -2400,13 +2427,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B117">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -2414,13 +2441,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B118">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -2428,13 +2455,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B119">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="C119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -2442,153 +2469,153 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B120">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="C120">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B121">
-        <v>1000</v>
+        <v>19</v>
       </c>
       <c r="C121">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B122">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="C122">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B123">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B124">
-        <v>1000000</v>
+        <v>40</v>
       </c>
       <c r="C124">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B125">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="C125">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B126">
-        <v>1000000000</v>
+        <v>60</v>
       </c>
       <c r="C126">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B127">
-        <v>1000000000</v>
+        <v>70</v>
       </c>
       <c r="C127">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B128">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B129">
-        <v>1000</v>
+        <v>90</v>
       </c>
       <c r="C129">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B130">
-        <v>1000000</v>
+        <v>100</v>
       </c>
       <c r="C130">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -2596,13 +2623,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B131">
-        <v>1000000000</v>
+        <v>1000</v>
       </c>
       <c r="C131">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -2610,13 +2637,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B132">
-        <v>1000000000000</v>
+        <v>1000</v>
       </c>
       <c r="C132">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -2624,13 +2651,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B133">
-        <v>1000000000000</v>
+        <v>1000</v>
       </c>
       <c r="C133">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D133">
         <v>1</v>
@@ -2638,13 +2665,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B134">
-        <v>1000000000000</v>
+        <v>1000000</v>
       </c>
       <c r="C134">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -2652,13 +2679,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B135">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="C135">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -2666,13 +2693,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B136">
-        <v>1000</v>
+        <v>1000000000</v>
       </c>
       <c r="C136">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -2680,13 +2707,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B137">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="C137">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -2694,13 +2721,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B138">
-        <v>1000000</v>
+        <v>12</v>
       </c>
       <c r="C138">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -2708,15 +2735,155 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B139">
+        <v>1000</v>
+      </c>
+      <c r="C139">
+        <v>4</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>124</v>
+      </c>
+      <c r="B140">
+        <v>1000000</v>
+      </c>
+      <c r="C140">
+        <v>5</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>125</v>
+      </c>
+      <c r="B141">
+        <v>1000000000</v>
+      </c>
+      <c r="C141">
+        <v>6</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>126</v>
+      </c>
+      <c r="B142">
+        <v>1000000000000</v>
+      </c>
+      <c r="C142">
+        <v>7</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>127</v>
+      </c>
+      <c r="B143">
+        <v>1000000000000</v>
+      </c>
+      <c r="C143">
+        <v>7</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>128</v>
+      </c>
+      <c r="B144">
+        <v>1000000000000</v>
+      </c>
+      <c r="C144">
+        <v>7</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>129</v>
+      </c>
+      <c r="B145">
+        <v>1000</v>
+      </c>
+      <c r="C145">
+        <v>4</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>130</v>
+      </c>
+      <c r="B146">
+        <v>1000</v>
+      </c>
+      <c r="C146">
+        <v>4</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>131</v>
+      </c>
+      <c r="B147">
+        <v>1000000</v>
+      </c>
+      <c r="C147">
+        <v>5</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>132</v>
+      </c>
+      <c r="B148">
+        <v>1000000</v>
+      </c>
+      <c r="C148">
+        <v>5</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>133</v>
+      </c>
+      <c r="B149">
         <v>100</v>
       </c>
-      <c r="C139">
+      <c r="C149">
         <v>3</v>
       </c>
-      <c r="D139">
+      <c r="D149">
         <v>0</v>
       </c>
     </row>

</xml_diff>